<commit_message>
Package and database updates.
</commit_message>
<xml_diff>
--- a/database/colorsExcelSheet.xlsx
+++ b/database/colorsExcelSheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="156">
   <si>
     <t>continent</t>
   </si>
@@ -145,24 +145,12 @@
     <t>American Samoa</t>
   </si>
   <si>
-    <t>North America</t>
-  </si>
-  <si>
-    <t>South America</t>
-  </si>
-  <si>
     <t>Australian Antarctic Claim</t>
   </si>
   <si>
     <t>Argentinian Antarctic Claim</t>
   </si>
   <si>
-    <t>Chilean Antarctic Claim</t>
-  </si>
-  <si>
-    <t>New Zealands Antarctic Claim</t>
-  </si>
-  <si>
     <t>Norwegian Antarctic Claim</t>
   </si>
   <si>
@@ -175,18 +163,6 @@
     <t>secondaryNotes</t>
   </si>
   <si>
-    <t>Colors from the unofficially proposed flag for the territory.</t>
-  </si>
-  <si>
-    <t>Colors from the unofficial flag of the Ross Dependancy.</t>
-  </si>
-  <si>
-    <t>Color used for the Afghanistan national cricket team.</t>
-  </si>
-  <si>
-    <t>Colors used in sports.</t>
-  </si>
-  <si>
     <t>#006230/#d30731/#fff</t>
   </si>
   <si>
@@ -332,6 +308,180 @@
   </si>
   <si>
     <t>hsl(197,100%,29%)/hsl(0,0%,0%)</t>
+  </si>
+  <si>
+    <t>Angola</t>
+  </si>
+  <si>
+    <t>Benin</t>
+  </si>
+  <si>
+    <t>Botswana</t>
+  </si>
+  <si>
+    <t>Burkina Faso</t>
+  </si>
+  <si>
+    <t>Burundi</t>
+  </si>
+  <si>
+    <t>Cameroon</t>
+  </si>
+  <si>
+    <t>Central African Republic</t>
+  </si>
+  <si>
+    <t>Chad</t>
+  </si>
+  <si>
+    <t>Comoros</t>
+  </si>
+  <si>
+    <t>AGO</t>
+  </si>
+  <si>
+    <t>BEN</t>
+  </si>
+  <si>
+    <t>BWA</t>
+  </si>
+  <si>
+    <t>BFA</t>
+  </si>
+  <si>
+    <t>BDI</t>
+  </si>
+  <si>
+    <t>CMR</t>
+  </si>
+  <si>
+    <t>CAF</t>
+  </si>
+  <si>
+    <t>TCD</t>
+  </si>
+  <si>
+    <t>COM</t>
+  </si>
+  <si>
+    <t>#cd022b/#000/#FC0</t>
+  </si>
+  <si>
+    <t>rgb(205,2,43)/rgb(0,0,0)/rgb(255,204,0)</t>
+  </si>
+  <si>
+    <t>hsl(348,98%,41%)/hsl(0,0%,0%)/hsl(48,100%,50%)</t>
+  </si>
+  <si>
+    <t>Colorsfromtheunofficiallyproposedflagfortheterritory.</t>
+  </si>
+  <si>
+    <t>ColorsfromtheunofficialflagoftheRossDependancy.</t>
+  </si>
+  <si>
+    <t>ColorusedfortheAfghanistannationalcricketteam.</t>
+  </si>
+  <si>
+    <t>NorthAmerica</t>
+  </si>
+  <si>
+    <t>SouthAmerica</t>
+  </si>
+  <si>
+    <t>Colorsusedinsports.</t>
+  </si>
+  <si>
+    <t>#008651/#fdd116/#e7112d</t>
+  </si>
+  <si>
+    <t>rgb(0,134,81)/rgb(253,209,22)/rgb(231,17,45)</t>
+  </si>
+  <si>
+    <t>#76a8db/#000/#fcfcfc</t>
+  </si>
+  <si>
+    <t>rgb(118,168,291)/rgb(0,0,0)/rgb(252,252,252)</t>
+  </si>
+  <si>
+    <t>#ef2b2d/#009e49/#fed116</t>
+  </si>
+  <si>
+    <t>rgb(239,43,45)/rgb(0,158,73)/rgb(254,209,22)</t>
+  </si>
+  <si>
+    <t>#cf0921/#fff/#18b737</t>
+  </si>
+  <si>
+    <t>rgb(207,9,33)/rgb(255,255,255)/rgb(24,183,55)</t>
+  </si>
+  <si>
+    <t>#007a5e/#ce1126/#fcd116</t>
+  </si>
+  <si>
+    <t>rgb(0,122,94)/rgb(206,17,38)/rgb(252,209,22)</t>
+  </si>
+  <si>
+    <t>Cape Verde</t>
+  </si>
+  <si>
+    <t>CPV</t>
+  </si>
+  <si>
+    <t>#013893/#fff/#ce1127/#ffc900</t>
+  </si>
+  <si>
+    <t>rgb(1,56,147)/rgb(255,255,255)/rgb(206,17,39)/rgb(255,201,0)</t>
+  </si>
+  <si>
+    <t>Chilean AntarcticClaim</t>
+  </si>
+  <si>
+    <t>NewZealands Antarctic Claim</t>
+  </si>
+  <si>
+    <t>hsl(156,100%,26%)/hsl(49,98%,54%)/hsl(352,86%,49%)</t>
+  </si>
+  <si>
+    <t>hsl(210,58%,66%)/hsl(0,0%,0%)/hsl(0,0%,99%)</t>
+  </si>
+  <si>
+    <t>hsl(359,86%,55%)/hsl(148,100%,31%)/hsl(48,99%,54%)</t>
+  </si>
+  <si>
+    <t>hsl(353,92%,42%)/hsl(0,0%,100%)/hsl(132,77%,41%)</t>
+  </si>
+  <si>
+    <t>hsl(166,100%,24%)/hsl(353,85%,44%)/hsl(49,97%,54%)</t>
+  </si>
+  <si>
+    <t>hsl(217,99%,29%)/hsl(0,0%,100%)/hsl(353,85%,44%)/hsl(47,100%,50%)</t>
+  </si>
+  <si>
+    <t>#08399c/#fff/#319400/#ffde00/#ef2900</t>
+  </si>
+  <si>
+    <t>rgb(8,57,156)/rgb(255,255,255)/rgb(49,148,0)/rgb(255,222,0)/rgb(239,41,0)</t>
+  </si>
+  <si>
+    <t>#002b7f/#fcd116/#ce1126</t>
+  </si>
+  <si>
+    <t>rgb(0,43,127)/rgb(252,209,22)/rgb(206,17,38)</t>
+  </si>
+  <si>
+    <t>#ffc718/#fff/#cf0921/#3775c5/3a8f30</t>
+  </si>
+  <si>
+    <t>rgb(255,199,24)/rgb(255,255,255)/rgb(207,9,33)/rgb(55,117,197)/rgb(58,143,48)</t>
+  </si>
+  <si>
+    <t>hsl(220,90%,32%)/hsl(0,0%,100%)/hsl(100,100%,29%)/hsl(52,100%,50%)/hsl(10,100%,47%)</t>
+  </si>
+  <si>
+    <t>hsl(220,100%,25%)/hsl(49,97%,54%)/hsl(353,85%,44%)</t>
+  </si>
+  <si>
+    <t>hsl(45,100%,55%)/hsl(0,0%,100%)/hsl(353,92%,42%)/hsl(214,56%,49%)/hsl(114,50%,37%)</t>
   </si>
 </sst>
 </file>
@@ -1168,10 +1318,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K14"/>
+  <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1180,9 +1330,9 @@
     <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="53.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="64.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="71.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="88.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="47.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="50.85546875" bestFit="1" customWidth="1"/>
@@ -1222,7 +1372,7 @@
         <v>12</v>
       </c>
       <c r="K1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -1239,337 +1389,567 @@
         <v>18</v>
       </c>
       <c r="E2" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="F2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="G2" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>45</v>
+        <v>98</v>
       </c>
       <c r="D3" t="s">
-        <v>30</v>
+        <v>107</v>
       </c>
       <c r="E3" t="s">
-        <v>58</v>
+        <v>116</v>
       </c>
       <c r="F3" t="s">
-        <v>73</v>
+        <v>117</v>
       </c>
       <c r="G3" t="s">
-        <v>90</v>
-      </c>
-      <c r="H3" t="s">
-        <v>59</v>
-      </c>
-      <c r="I3" t="s">
-        <v>74</v>
-      </c>
-      <c r="J3" t="s">
-        <v>91</v>
-      </c>
-      <c r="K3" t="s">
-        <v>53</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>46</v>
+        <v>99</v>
       </c>
       <c r="D4" t="s">
-        <v>31</v>
+        <v>108</v>
       </c>
       <c r="E4" t="s">
-        <v>62</v>
+        <v>125</v>
       </c>
       <c r="F4" t="s">
-        <v>75</v>
-      </c>
-      <c r="G4" t="s">
-        <v>92</v>
+        <v>126</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>47</v>
+        <v>100</v>
       </c>
       <c r="D5" t="s">
-        <v>32</v>
+        <v>109</v>
       </c>
       <c r="E5" t="s">
-        <v>63</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>76</v>
+        <v>127</v>
+      </c>
+      <c r="F5" t="s">
+        <v>128</v>
       </c>
       <c r="G5" t="s">
-        <v>93</v>
+        <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D6" t="s">
-        <v>33</v>
+        <v>110</v>
       </c>
       <c r="E6" t="s">
-        <v>64</v>
+        <v>129</v>
       </c>
       <c r="F6" t="s">
-        <v>77</v>
+        <v>130</v>
       </c>
       <c r="G6" t="s">
-        <v>94</v>
+        <v>143</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>48</v>
+        <v>102</v>
       </c>
       <c r="D7" t="s">
-        <v>34</v>
+        <v>111</v>
       </c>
       <c r="E7" t="s">
-        <v>65</v>
+        <v>131</v>
       </c>
       <c r="F7" t="s">
-        <v>78</v>
+        <v>132</v>
       </c>
       <c r="G7" t="s">
-        <v>95</v>
-      </c>
-      <c r="H7" t="s">
-        <v>60</v>
-      </c>
-      <c r="I7" t="s">
-        <v>79</v>
-      </c>
-      <c r="J7" t="s">
-        <v>96</v>
-      </c>
-      <c r="K7" t="s">
-        <v>54</v>
+        <v>144</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>49</v>
+        <v>103</v>
       </c>
       <c r="D8" t="s">
-        <v>35</v>
+        <v>112</v>
       </c>
       <c r="E8" t="s">
-        <v>66</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>80</v>
+        <v>133</v>
+      </c>
+      <c r="F8" t="s">
+        <v>134</v>
       </c>
       <c r="G8" t="s">
-        <v>97</v>
+        <v>145</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>50</v>
+        <v>135</v>
       </c>
       <c r="D9" t="s">
-        <v>36</v>
+        <v>136</v>
       </c>
       <c r="E9" t="s">
-        <v>61</v>
+        <v>137</v>
       </c>
       <c r="F9" t="s">
-        <v>81</v>
+        <v>138</v>
       </c>
       <c r="G9" t="s">
-        <v>98</v>
+        <v>146</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>104</v>
       </c>
       <c r="D10" t="s">
-        <v>21</v>
+        <v>113</v>
       </c>
       <c r="E10" t="s">
-        <v>67</v>
+        <v>147</v>
       </c>
       <c r="F10" t="s">
-        <v>82</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="H10" t="s">
-        <v>22</v>
-      </c>
-      <c r="I10" t="s">
-        <v>83</v>
-      </c>
-      <c r="J10" t="s">
-        <v>100</v>
-      </c>
-      <c r="K10" t="s">
-        <v>55</v>
+        <v>148</v>
+      </c>
+      <c r="G10" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>23</v>
+        <v>105</v>
       </c>
       <c r="D11" t="s">
-        <v>24</v>
+        <v>114</v>
       </c>
       <c r="E11" t="s">
-        <v>68</v>
+        <v>149</v>
       </c>
       <c r="F11" t="s">
-        <v>84</v>
+        <v>150</v>
       </c>
       <c r="G11" t="s">
-        <v>101</v>
+        <v>154</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>43</v>
+        <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>9</v>
+        <v>106</v>
       </c>
       <c r="D12" t="s">
-        <v>19</v>
+        <v>115</v>
       </c>
       <c r="E12" t="s">
-        <v>69</v>
+        <v>151</v>
       </c>
       <c r="F12" t="s">
-        <v>85</v>
+        <v>152</v>
       </c>
       <c r="G12" t="s">
-        <v>102</v>
+        <v>155</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C13" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D13" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E13" t="s">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="F13" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
       <c r="G13" t="s">
-        <v>103</v>
+        <v>82</v>
+      </c>
+      <c r="H13" t="s">
+        <v>51</v>
+      </c>
+      <c r="I13" t="s">
+        <v>66</v>
+      </c>
+      <c r="J13" t="s">
+        <v>83</v>
+      </c>
+      <c r="K13" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" t="s">
         <v>44</v>
       </c>
-      <c r="B14" t="s">
+      <c r="D14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" t="s">
+        <v>54</v>
+      </c>
+      <c r="F14" t="s">
+        <v>67</v>
+      </c>
+      <c r="G14" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" t="s">
+        <v>139</v>
+      </c>
+      <c r="D15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E15" t="s">
+        <v>55</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G15" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16" t="s">
+        <v>33</v>
+      </c>
+      <c r="E16" t="s">
+        <v>56</v>
+      </c>
+      <c r="F16" t="s">
+        <v>69</v>
+      </c>
+      <c r="G16" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" t="s">
+        <v>140</v>
+      </c>
+      <c r="D17" t="s">
+        <v>34</v>
+      </c>
+      <c r="E17" t="s">
+        <v>57</v>
+      </c>
+      <c r="F17" t="s">
+        <v>70</v>
+      </c>
+      <c r="G17" t="s">
+        <v>87</v>
+      </c>
+      <c r="H17" t="s">
+        <v>52</v>
+      </c>
+      <c r="I17" t="s">
+        <v>71</v>
+      </c>
+      <c r="J17" t="s">
+        <v>88</v>
+      </c>
+      <c r="K17" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" t="s">
+        <v>58</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G18" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" t="s">
+        <v>46</v>
+      </c>
+      <c r="D19" t="s">
+        <v>36</v>
+      </c>
+      <c r="E19" t="s">
+        <v>53</v>
+      </c>
+      <c r="F19" t="s">
+        <v>73</v>
+      </c>
+      <c r="G19" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" t="s">
+        <v>21</v>
+      </c>
+      <c r="E20" t="s">
+        <v>59</v>
+      </c>
+      <c r="F20" t="s">
+        <v>74</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H20" t="s">
+        <v>22</v>
+      </c>
+      <c r="I20" t="s">
+        <v>75</v>
+      </c>
+      <c r="J20" t="s">
+        <v>92</v>
+      </c>
+      <c r="K20" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21" t="s">
+        <v>60</v>
+      </c>
+      <c r="F21" t="s">
+        <v>76</v>
+      </c>
+      <c r="G21" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>122</v>
+      </c>
+      <c r="B22" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" t="s">
+        <v>19</v>
+      </c>
+      <c r="E22" t="s">
+        <v>61</v>
+      </c>
+      <c r="F22" t="s">
+        <v>77</v>
+      </c>
+      <c r="G22" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" t="s">
+        <v>42</v>
+      </c>
+      <c r="D23" t="s">
+        <v>27</v>
+      </c>
+      <c r="E23" t="s">
+        <v>62</v>
+      </c>
+      <c r="F23" t="s">
+        <v>78</v>
+      </c>
+      <c r="G23" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>123</v>
+      </c>
+      <c r="B24" t="s">
         <v>13</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C24" t="s">
         <v>14</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D24" t="s">
         <v>20</v>
       </c>
-      <c r="E14" t="s">
-        <v>71</v>
-      </c>
-      <c r="F14" t="s">
-        <v>87</v>
-      </c>
-      <c r="G14" t="s">
-        <v>104</v>
-      </c>
-      <c r="H14" t="s">
+      <c r="E24" t="s">
+        <v>63</v>
+      </c>
+      <c r="F24" t="s">
+        <v>79</v>
+      </c>
+      <c r="G24" t="s">
+        <v>96</v>
+      </c>
+      <c r="H24" t="s">
         <v>41</v>
       </c>
-      <c r="I14" t="s">
-        <v>88</v>
-      </c>
-      <c r="J14" t="s">
-        <v>105</v>
-      </c>
-      <c r="K14" t="s">
-        <v>56</v>
+      <c r="I24" t="s">
+        <v>80</v>
+      </c>
+      <c r="J24" t="s">
+        <v>97</v>
+      </c>
+      <c r="K24" t="s">
+        <v>124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Restructured files, added gulp, eslint, browserslist, express router, ejs. Setup css and linting gulp tasks.
</commit_message>
<xml_diff>
--- a/database/colorsExcelSheet.xlsx
+++ b/database/colorsExcelSheet.xlsx
@@ -436,9 +436,6 @@
     <t>Chilean AntarcticClaim</t>
   </si>
   <si>
-    <t>NewZealands Antarctic Claim</t>
-  </si>
-  <si>
     <t>hsl(156,100%,26%)/hsl(49,98%,54%)/hsl(352,86%,49%)</t>
   </si>
   <si>
@@ -482,6 +479,9 @@
   </si>
   <si>
     <t>hsl(45,100%,55%)/hsl(0,0%,100%)/hsl(353,92%,42%)/hsl(214,56%,49%)/hsl(114,50%,37%)</t>
+  </si>
+  <si>
+    <t>New Zealands Antarctic Claim</t>
   </si>
 </sst>
 </file>
@@ -1321,7 +1321,7 @@
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1441,7 +1441,7 @@
         <v>126</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -1464,7 +1464,7 @@
         <v>128</v>
       </c>
       <c r="G5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -1487,7 +1487,7 @@
         <v>130</v>
       </c>
       <c r="G6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -1510,7 +1510,7 @@
         <v>132</v>
       </c>
       <c r="G7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -1533,7 +1533,7 @@
         <v>134</v>
       </c>
       <c r="G8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -1556,7 +1556,7 @@
         <v>138</v>
       </c>
       <c r="G9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -1573,13 +1573,13 @@
         <v>113</v>
       </c>
       <c r="E10" t="s">
+        <v>146</v>
+      </c>
+      <c r="F10" t="s">
         <v>147</v>
       </c>
-      <c r="F10" t="s">
-        <v>148</v>
-      </c>
       <c r="G10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -1596,13 +1596,13 @@
         <v>114</v>
       </c>
       <c r="E11" t="s">
+        <v>148</v>
+      </c>
+      <c r="F11" t="s">
         <v>149</v>
       </c>
-      <c r="F11" t="s">
-        <v>150</v>
-      </c>
       <c r="G11" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -1619,13 +1619,13 @@
         <v>115</v>
       </c>
       <c r="E12" t="s">
+        <v>150</v>
+      </c>
+      <c r="F12" t="s">
         <v>151</v>
       </c>
-      <c r="F12" t="s">
-        <v>152</v>
-      </c>
       <c r="G12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -1740,7 +1740,7 @@
         <v>29</v>
       </c>
       <c r="C17" t="s">
-        <v>140</v>
+        <v>155</v>
       </c>
       <c r="D17" t="s">
         <v>34</v>

</xml_diff>